<commit_message>
Added Prospectus supp figs
</commit_message>
<xml_diff>
--- a/kaiju/inulinase/tax_summarized/metabolism/family.sum.xlsx
+++ b/kaiju/inulinase/tax_summarized/metabolism/family.sum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\OneDrive\Documents\GitHub\Carb_CRDS\kaiju\inulinase\tax_summarized\metabolism\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/kaiju/inulinase/tax_summarized/metabolism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C3A41ABA-2115-4701-AAA0-DC76122BB81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:40009_{C3A41ABA-2115-4701-AAA0-DC76122BB81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1150EBF4-0492-4923-BDC9-DA16FA31224D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="family.sum" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="72">
   <si>
     <t>Domain</t>
   </si>
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,7 +378,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -567,6 +567,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,10 +737,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -782,6 +789,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1089,27 +1101,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1170,7 +1182,7 @@
         <v>1.5447957999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1199,39 +1211,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>13.624056169999999</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>3.210773155</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>13.429685599999999</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="3">
         <v>4.641153096</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>0.15166543299999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1289,39 +1298,36 @@
         <v>1.5708996999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>9.6504873329999992</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>1.6446904710000001</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>9.2091727999999993</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <v>2.3672341889999999</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>2.2255199999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1382,7 +1388,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>3.6973616000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1443,7 +1449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>6.8306E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1530,7 +1536,7 @@
         <v>1.9880800000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1559,7 +1565,7 @@
         <v>7.4184000000000003E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1588,7 +1594,7 @@
         <v>7.4184000000000003E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1617,7 +1623,7 @@
         <v>0.10879570199999999</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1646,7 +1652,7 @@
         <v>9.3895999999999997E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>4.6947999999999998E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1704,7 +1710,7 @@
         <v>1.9339194000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1733,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>9.7238375000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1791,39 +1797,36 @@
         <v>3.9049671000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>0.57008083300000001</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>0.19715898800000001</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
         <v>0</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="1">
         <v>0</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>8.9201799999999998E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -1881,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>64</v>
       </c>
@@ -1910,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>70</v>
       </c>

</xml_diff>